<commit_message>
final commit from my side
</commit_message>
<xml_diff>
--- a/csp301/Final Analysis.xlsx
+++ b/csp301/Final Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="booksGraphAnalysis" sheetId="1" r:id="rId1"/>
@@ -5950,11 +5950,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75492352"/>
-        <c:axId val="75494528"/>
+        <c:axId val="97774592"/>
+        <c:axId val="97776768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75492352"/>
+        <c:axId val="97774592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5983,12 +5983,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75494528"/>
+        <c:crossAx val="97776768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75494528"/>
+        <c:axId val="97776768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6018,7 +6018,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75492352"/>
+        <c:crossAx val="97774592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15051,11 +15051,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="76032256"/>
-        <c:axId val="76042624"/>
+        <c:axId val="99756288"/>
+        <c:axId val="99766656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76032256"/>
+        <c:axId val="99756288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15084,12 +15084,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76042624"/>
+        <c:crossAx val="99766656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76042624"/>
+        <c:axId val="99766656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15119,7 +15119,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76032256"/>
+        <c:crossAx val="99756288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15498,11 +15498,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16398,6 +16398,18 @@
         <v>0.75732807511015499</v>
       </c>
     </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="1">
+        <f>MIN(D2:D52)</f>
+        <v>0.34920634920634902</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="1">
+        <f>MAX(D3:D52)</f>
+        <v>0.43310657596371799</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -16408,9 +16420,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19680,7 +19692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1491"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>

</xml_diff>